<commit_message>
Had some random column making it funky
</commit_message>
<xml_diff>
--- a/vignettes/Wide data example.xlsx
+++ b/vignettes/Wide data example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LADData\toxEval\vignettes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B832CAD-D4F2-437D-BA26-478BF7BDA726}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6E803E-E9B4-44B4-8802-04D7DB0AFDB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="376" yWindow="376" windowWidth="18031" windowHeight="10518" xr2:uid="{B268D3CA-A042-D94E-A71E-6DD630BC48E0}"/>
+    <workbookView xWindow="714" yWindow="614" windowWidth="20360" windowHeight="13536" xr2:uid="{B268D3CA-A042-D94E-A71E-6DD630BC48E0}"/>
   </bookViews>
   <sheets>
     <sheet name="data_from_lab" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
   <si>
     <t>1912-24-9</t>
   </si>
@@ -473,15 +473,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3281CD6-97E3-2E44-8877-754C17A6D27E}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.65" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -498,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -526,11 +526,8 @@
       <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -538,7 +535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -569,11 +566,8 @@
       <c r="J5">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -604,11 +598,8 @@
       <c r="J6">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -639,11 +630,8 @@
       <c r="J7">
         <v>0.08</v>
       </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -674,11 +662,8 @@
       <c r="J8">
         <v>0.08</v>
       </c>
-      <c r="K8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -709,11 +694,8 @@
       <c r="J9">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -744,11 +726,8 @@
       <c r="J10">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -779,11 +758,8 @@
       <c r="J11">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -814,11 +790,8 @@
       <c r="J12">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -849,11 +822,8 @@
       <c r="J13">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -884,11 +854,8 @@
       <c r="J14">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -919,11 +886,8 @@
       <c r="J15">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -953,9 +917,6 @@
       </c>
       <c r="J16">
         <v>8.3000000000000001E-3</v>
-      </c>
-      <c r="K16" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>